<commit_message>
made changes in repository
</commit_message>
<xml_diff>
--- a/com.automation.selenium/src/test/resources/TestData/SysadminTestData.xlsx
+++ b/com.automation.selenium/src/test/resources/TestData/SysadminTestData.xlsx
@@ -544,8 +544,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D27" sqref="D27"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Changes done in testng.xml
</commit_message>
<xml_diff>
--- a/com.automation.selenium/src/test/resources/TestData/SysadminTestData.xlsx
+++ b/com.automation.selenium/src/test/resources/TestData/SysadminTestData.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="55">
   <si>
     <t>TC ID</t>
   </si>
@@ -117,9 +117,6 @@
     <t>S008</t>
   </si>
   <si>
-    <t>name@gmail.com</t>
-  </si>
-  <si>
     <t>S009</t>
   </si>
   <si>
@@ -129,9 +126,6 @@
     <t>vY78_h$ia</t>
   </si>
   <si>
-    <t>S011</t>
-  </si>
-  <si>
     <t>Downloadlogs</t>
   </si>
   <si>
@@ -159,13 +153,34 @@
     <t>CleanRequest</t>
   </si>
   <si>
-    <t>name1</t>
-  </si>
-  <si>
-    <t>S017</t>
-  </si>
-  <si>
     <t>tej</t>
+  </si>
+  <si>
+    <t>tej@gmail.com</t>
+  </si>
+  <si>
+    <t>licensePath</t>
+  </si>
+  <si>
+    <t>\licenseFile\Tejaswini_DEVELOPMENT.lic</t>
+  </si>
+  <si>
+    <t>S014</t>
+  </si>
+  <si>
+    <t>S015</t>
+  </si>
+  <si>
+    <t>tej54</t>
+  </si>
+  <si>
+    <t>name45@gmail.com</t>
+  </si>
+  <si>
+    <t>changePassword</t>
+  </si>
+  <si>
+    <t>OldPassword</t>
   </si>
 </sst>
 </file>
@@ -544,8 +559,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D23" sqref="D23"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -572,21 +587,27 @@
         <v>2</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>18</v>
+        <v>53</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>37</v>
+        <v>3</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="D2" s="4" t="s">
+      <c r="C2" s="4" t="s">
         <v>19</v>
+      </c>
+      <c r="D2" s="7">
+        <v>0</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
@@ -594,50 +615,43 @@
         <v>0</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>2</v>
+        <v>14</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C4" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="D4" s="7"/>
+        <v>6</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B6" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B6" s="2" t="s">
         <v>10</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>26</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
@@ -645,15 +659,49 @@
         <v>0</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>9</v>
+        <v>12</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="G7" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="H7" s="2" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>10</v>
+        <v>24</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="E8" s="4"/>
+      <c r="F8" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="G8" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="H8" s="7" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
@@ -661,49 +709,27 @@
         <v>0</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>13</v>
+        <v>2</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="E9" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="F9" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="G9" s="2" t="s">
         <v>17</v>
-      </c>
-      <c r="H9" s="2" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="B10" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="C10" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="D10" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="E10" s="4"/>
-      <c r="F10" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="G10" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="H10" s="7" t="s">
-        <v>19</v>
+        <v>21</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="D10" s="5" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
@@ -711,27 +737,15 @@
         <v>0</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="C11" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="D11" s="2" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="B12" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="C12" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="D12" s="5" t="s">
-        <v>20</v>
+        <v>23</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
@@ -739,15 +753,57 @@
         <v>0</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>22</v>
+        <v>30</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E13" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="F13" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="G13" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="H13" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="I13" s="2" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
-        <v>23</v>
+        <v>29</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>24</v>
+        <v>38</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="E14" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="F14" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="G14" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="H14" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="I14" s="7" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
@@ -755,193 +811,161 @@
         <v>0</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>30</v>
+        <v>16</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>12</v>
+        <v>2</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="E15" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="F15" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="G15" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="H15" s="2" t="s">
         <v>17</v>
-      </c>
-      <c r="I15" s="2" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="B16" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="B16" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="C16" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="D16" s="7" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="B18" s="6" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A21" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B21" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="C16" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="D16" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="E16" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="F16" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="G16" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="H16" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="I16" s="7" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B17" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="C17" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="D17" s="2" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="B18" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="C18" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="D18" s="7" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B19" s="2" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="B20" s="6" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A21" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B21" s="2" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="B22" s="2" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B22" s="4" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="B24" s="4" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B24" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+      <c r="C25" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D25"/>
+      <c r="E25"/>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="B26" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="B26" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C26" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="D26"/>
+      <c r="E26"/>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B27" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C27" s="2" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B27" t="s">
+        <v>47</v>
+      </c>
+      <c r="C27"/>
+      <c r="D27"/>
+      <c r="E27"/>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="B28" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="B28" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="C28" s="4" t="s">
-        <v>19</v>
-      </c>
+      <c r="C28"/>
+      <c r="D28"/>
+      <c r="E28"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="F10" r:id="rId1"/>
-    <hyperlink ref="G10" r:id="rId2"/>
-    <hyperlink ref="H10" r:id="rId3"/>
-    <hyperlink ref="C12" r:id="rId4"/>
-    <hyperlink ref="D12" r:id="rId5"/>
-    <hyperlink ref="B12" r:id="rId6"/>
-    <hyperlink ref="G16" r:id="rId7"/>
-    <hyperlink ref="H16" r:id="rId8"/>
-    <hyperlink ref="I16" r:id="rId9"/>
-    <hyperlink ref="C18" r:id="rId10"/>
-    <hyperlink ref="D18" r:id="rId11"/>
-    <hyperlink ref="B18" r:id="rId12"/>
-    <hyperlink ref="B20" r:id="rId13" display="name@gmail.com"/>
-    <hyperlink ref="C2" r:id="rId14" display="Vyom@123"/>
-    <hyperlink ref="D2" r:id="rId15"/>
-    <hyperlink ref="B24" r:id="rId16" display="http://10.51.29.24:8080"/>
-    <hyperlink ref="C4" r:id="rId17"/>
-    <hyperlink ref="C28" r:id="rId18"/>
+    <hyperlink ref="F8" r:id="rId1"/>
+    <hyperlink ref="G8" r:id="rId2"/>
+    <hyperlink ref="H8" r:id="rId3"/>
+    <hyperlink ref="C10" r:id="rId4"/>
+    <hyperlink ref="D10" r:id="rId5"/>
+    <hyperlink ref="B10" r:id="rId6"/>
+    <hyperlink ref="G14" r:id="rId7"/>
+    <hyperlink ref="H14" r:id="rId8"/>
+    <hyperlink ref="I14" r:id="rId9"/>
+    <hyperlink ref="C16" r:id="rId10"/>
+    <hyperlink ref="D16" r:id="rId11"/>
+    <hyperlink ref="B16" r:id="rId12"/>
+    <hyperlink ref="B18" r:id="rId13" display="name@gmail.com"/>
+    <hyperlink ref="B22" r:id="rId14" display="http://10.51.29.24:8080"/>
+    <hyperlink ref="F14" r:id="rId15"/>
+    <hyperlink ref="C26" r:id="rId16"/>
+    <hyperlink ref="B28" r:id="rId17" display="\\licenseFile\\Tejaswini_DEVELOPMENT.lic"/>
+    <hyperlink ref="E2" r:id="rId18" display="Vyom@123"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId19"/>
@@ -950,12 +974,32 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:C4"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A21" sqref="A21"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="2"/>
+      <c r="B1" s="2"/>
+      <c r="C1" s="2"/>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="2"/>
+      <c r="B2" s="2"/>
+      <c r="C2" s="4"/>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="2"/>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="2"/>
+      <c r="B4" s="4"/>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>